<commit_message>
GDD and Asset List Update
Updated both to include other categories forgotten and write the game is to be a windowed game.
</commit_message>
<xml_diff>
--- a/Design Documents/Asset List.xlsx
+++ b/Design Documents/Asset List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kieran\Desktop\Games Unity\Personal\Layer Up\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F45CA3-2456-4D54-87E4-4A2F0A0EC304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FF3AE4-3F5B-44D7-AF61-35CB82A3750D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12504" xr2:uid="{58F35872-8E95-4493-B93C-0F6E0473205D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" xr2:uid="{58F35872-8E95-4493-B93C-0F6E0473205D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Assets List</t>
   </si>
@@ -108,11 +108,6 @@
 Looking at anime character for it maybe.</t>
   </si>
   <si>
-    <t xml:space="preserve">The game itself uses speed runner music but realised probs doesn't fit theme as there need to be a reason it loops.
-Check binding of Issac for how they do music and then select from pack.
-</t>
-  </si>
-  <si>
     <t>https://drive.google.com/drive/folders/1aV9m2S6_pb1bOSTbW7qG8IN_3aAU18Vu
 https://assetstore.unity.com/packages/audio/music/electronic/my-little-bots-crazy-music-for-robots-asset-pack-196365 &lt;- Sounds fitting for speed running repeating fast paced levels.</t>
   </si>
@@ -125,6 +120,50 @@
   </si>
   <si>
     <t>Free packs and base 2d platformer asset.</t>
+  </si>
+  <si>
+    <t>Game Play Assets</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Icons</t>
+  </si>
+  <si>
+    <t>Curser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the gameplay icon to play the game. This will be using:
+GUI PRO Kit - Casual Game
+GUI PRO Kit - Fantasy RPG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the mouse to play the game. This will be using:
+GUI PRO Kit - Casual Game
+GUI PRO Kit - Fantasy RPG </t>
+  </si>
+  <si>
+    <t>Level Up Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using the following to make:
+GUI PRO Kit - Casual Game
+GUI PRO Kit - Fantasy RPG </t>
+  </si>
+  <si>
+    <t>In Game Timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The game itself uses speed runner music but realised probs doesn't fit theme as there need to be a reason it loops.
+Check binding of Issac for how they do music and then select from pack Jay Ray gave us.
+</t>
+  </si>
+  <si>
+    <t>Platform Breaking Effects</t>
+  </si>
+  <si>
+    <t>Will use Rayfire to pre break platforms and have the effect fo breaking.</t>
   </si>
 </sst>
 </file>
@@ -526,18 +565,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D089ACAB-5765-4938-845C-9B36122EE218}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.88671875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64" style="1" customWidth="1"/>
+    <col min="4" max="4" width="134.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -551,7 +589,7 @@
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -585,66 +623,115 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>21</v>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -653,8 +740,8 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://www.gameuidatabase.com/uploads/The-End-Is-Nigh07052020-054640-96550.jpg" xr:uid="{B526C87B-BD2F-42CD-85BC-9BD969A75EBD}"/>
-    <hyperlink ref="D11" r:id="rId2" display="https://drive.google.com/drive/folders/1aV9m2S6_pb1bOSTbW7qG8IN_3aAU18Vu_x000a_" xr:uid="{0486C94C-C995-4D85-9D89-9C88C0C9FEE9}"/>
+    <hyperlink ref="D7" r:id="rId1" display="https://www.gameuidatabase.com/uploads/The-End-Is-Nigh07052020-054640-96550.jpg" xr:uid="{B526C87B-BD2F-42CD-85BC-9BD969A75EBD}"/>
+    <hyperlink ref="D14" r:id="rId2" display="https://drive.google.com/drive/folders/1aV9m2S6_pb1bOSTbW7qG8IN_3aAU18Vu_x000a_" xr:uid="{0486C94C-C995-4D85-9D89-9C88C0C9FEE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>

</xml_diff>